<commit_message>
19th Jan,2013 ... 2
</commit_message>
<xml_diff>
--- a/Repository/Schematic Library/Database_Library/components.xlsx
+++ b/Repository/Schematic Library/Database_Library/components.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8126" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8129" uniqueCount="1218">
   <si>
     <t>Part Number</t>
   </si>
@@ -3659,6 +3659,18 @@
   </si>
   <si>
     <t>SPDT_Power_L102021ML04Q_Thru-Hole</t>
+  </si>
+  <si>
+    <t>GainBlock_RFMD_SGA6489_PCB</t>
+  </si>
+  <si>
+    <t>NMOS_Fairchild_FDV301_SOT23-3</t>
+  </si>
+  <si>
+    <t>TCXO_KYOCERA_KT2520Y40000ECV28TBA_PCB-6PIN</t>
+  </si>
+  <si>
+    <t>ZYNQ_xc7z020clg484pkg_BGA-484</t>
   </si>
 </sst>
 </file>
@@ -17932,8 +17944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E66"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18613,18 +18625,22 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:8" s="20" customFormat="1">
+      <c r="A13" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="21" t="s">
         <v>781</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="22" t="s">
         <v>782</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="23"/>
+      <c r="E13" s="19" t="s">
         <v>783</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="20" customFormat="1">
@@ -18843,18 +18859,22 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:7" s="20" customFormat="1">
+      <c r="A26" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="21" t="s">
         <v>1117</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="21" t="s">
         <v>1118</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="23"/>
+      <c r="E26" s="24" t="s">
         <v>1119</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="20" customFormat="1">
@@ -19409,21 +19429,24 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="6" t="s">
+    <row r="58" spans="1:6" s="20" customFormat="1">
+      <c r="A58" s="21" t="s">
         <v>852</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="21" t="s">
         <v>853</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="21" t="s">
         <v>854</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="23" t="s">
         <v>855</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="19" t="s">
         <v>856</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="20" customFormat="1">
@@ -19522,22 +19545,22 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:6" s="20" customFormat="1" ht="15.75">
+      <c r="A64" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="16" t="s">
         <v>423</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="1" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F64" s="13" t="s">
-        <v>101</v>
+      <c r="F64" s="19" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="20" customFormat="1">

</xml_diff>

<commit_message>
19th Jan,2013 ... 3
</commit_message>
<xml_diff>
--- a/Repository/Schematic Library/Database_Library/components.xlsx
+++ b/Repository/Schematic Library/Database_Library/components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4117,8 +4117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G700"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A361" sqref="A361:XFD673"/>
+    <sheetView topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17944,8 +17944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19892,7 +19892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:F52"/>
     </sheetView>
   </sheetViews>
@@ -20955,8 +20955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H585"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>